<commit_message>
add Unit data and Image
</commit_message>
<xml_diff>
--- a/Plan/GameData/UnitDatabase_v03.xlsx
+++ b/Plan/GameData/UnitDatabase_v03.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\min\Projects\HotSix\Plan\GameData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김효빈\Documents\GitHub\HotSix\Plan\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD23450C-E6EE-4A08-AE24-9151FF19F63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F7793E-B28B-4F78-B6C2-8DB6FBD6E828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37340" yWindow="2920" windowWidth="23190" windowHeight="18160" xr2:uid="{0AD19C01-F545-4496-A2AF-5430239E61B1}"/>
+    <workbookView xWindow="1215" yWindow="840" windowWidth="25725" windowHeight="13800" activeTab="3" xr2:uid="{0AD19C01-F545-4496-A2AF-5430239E61B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="106">
   <si>
     <t>Move Speed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -387,13 +387,75 @@
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>항상 갈라지는 등딱지 때문에 고민이 많던 투카 용병단은 어느 날 빈 대포를 찾게 됩니다. 들어가보니 딱 맞는 것이 아니겠어요? 아, 어떻게 들어갔는지는 물어보지 마세요. 공격을 무서워해서 숨는 습성이 있습니다. 대신 높은 체력과 방어력으로 팀을 적의 공격으로부터 막아줍니다</t>
+  </si>
+  <si>
+    <t>덕배 용병단은 곰처럼 몸이 커지고 싶었습니다. 운 좋게 얻은 곰 모양의 옷에 맞춰 열심히 운동한 결과 그들은 곰이 되었습니다! 아니, 정확하게 말하면 곰처럼 변했다고 해야할까요? 단단한 몸으로 한 번에 강력한 공격을 합니다</t>
+  </si>
+  <si>
+    <t>람지 쌍검단은 쌍검을 쓰는 용맹한 전사들입니다! 작지만 재빠른 이동과 공격으로 적의 혼을 빼놓지요! 한 번에 두 번의 공격을 합니다</t>
+  </si>
+  <si>
+    <t>금호 창술단은 원래 오토바이를 타고 다니던 불량한 무리였습니다. 하지만 창을 배우고 난 뒤 건실하게 살아가고 있습니다. 긴 창을 이용하여 조금 더 멀리서 강한 공격을 합니다</t>
+  </si>
+  <si>
+    <t>아라 궁수단은 활을 쏘는 연습을 매일 하는 용병단입니다. 전쟁에 나가기 전에 자신의 단원의 머리 위의 모자에 화살을 맞추는 의식을 치루는 것으로 유명합니다. 잘못 맞으면 어떡하냐구요? 그럴 일은 없습니다~ 활을 이용하여 원거리에서 적을 공격합니다</t>
+  </si>
+  <si>
+    <t>카마 마법사단은 다양한 마법을 연구하는 용병단입니다. 이젠 그들의 장기를 활용하여 엄청난 마법을 보여주려 합니다! 전기 구체를 발사하여 원거리에서 공격합니다</t>
+  </si>
+  <si>
+    <t>홀리 성직자단은 왕국의 안녕과 평화를 기원하는 공동체입니다. 전투에 참여하고 싶지 않았지만 세계의 균형을 위해 전투에 참여하였습니다 공격을 하지 않고 일정 범위 내의 아군에게 체력, 방어력 증가 버프를 부여합니다</t>
+  </si>
+  <si>
+    <t>바빗 음악단은 여유롭게 음악을 즐기는 토끼들이 뭉친 집단입니다. 사람들이 많은 곳에서 연주를 하는 것을 즐기던 토끼들이 이번 전투에서 자신들이 도움을 줄 수 있다는 것을 깨닫고 기꺼이 참여했습니다! 일정 범위 내의 아군에게 공속, 이속 증가 버프를 제공합니다. 적이 근접하면 약한 공격을 합니다</t>
+  </si>
+  <si>
+    <t>고릴라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저가 연속으로 문제를 틀릴시 나타난다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reaper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Peace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테이저</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피스는 왕국의 평화를 책임지는 믿음직한 비둘기입니다. 순백의 날개를 펼치면 아군들은 기쁨에 가득찹니다! 아군 유닛에게 일정 시간 무적 효과를 부여합니다</t>
+  </si>
+  <si>
+    <t>테이저는 왕국의 위협을 감시하는 하늘의 지킴이입니다. 위험한 현장에는 바람같이 나타나 적을 위협하여 아군을 지킵니다! 적 유닛에게 일정 시간 스턴 효과를 부여합니다</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +481,12 @@
       <sz val="11"/>
       <color rgb="FF202124"/>
       <name val="Inherit"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -603,7 +671,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -649,6 +717,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -670,9 +741,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -681,6 +749,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -998,36 +1069,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECDDCD4-1D27-4FE4-92BB-9026CE350CFB}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="15.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.58203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.08203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.875" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.83203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.58203125" style="1"/>
+    <col min="9" max="9" width="21.875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
@@ -1105,7 +1176,7 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1126,7 +1197,7 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="20"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
@@ -1145,7 +1216,7 @@
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="21"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -1164,17 +1235,17 @@
       <c r="I7" s="2"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
@@ -1330,16 +1401,16 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
       <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:9">
@@ -1432,16 +1503,16 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="7">
@@ -1546,28 +1617,28 @@
       <c r="H32" s="2"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="7">
@@ -1654,16 +1725,16 @@
       <c r="H42" s="4"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="7">
@@ -1750,16 +1821,16 @@
       <c r="H48" s="4"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="7">
@@ -1846,16 +1917,16 @@
       <c r="H54" s="4"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="16"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="7">
@@ -1942,16 +2013,16 @@
       <c r="H60" s="4"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="15" t="s">
+      <c r="A62" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="16"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="7">
@@ -2038,16 +2109,16 @@
       <c r="H66" s="4"/>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="15" t="s">
+      <c r="A68" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B68" s="16"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
-      <c r="H68" s="16"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="17"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="7">
@@ -2134,16 +2205,16 @@
       <c r="H72" s="4"/>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="15" t="s">
+      <c r="A74" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
-      <c r="D74" s="16"/>
-      <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="16"/>
-      <c r="H74" s="16"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="7">
@@ -2248,16 +2319,16 @@
       <c r="H79" s="4"/>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="15" t="s">
+      <c r="A81" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B81" s="16"/>
-      <c r="C81" s="16"/>
-      <c r="D81" s="16"/>
-      <c r="E81" s="16"/>
-      <c r="F81" s="16"/>
-      <c r="G81" s="16"/>
-      <c r="H81" s="16"/>
+      <c r="B81" s="17"/>
+      <c r="C81" s="17"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="17"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="17"/>
+      <c r="H81" s="17"/>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" s="7">
@@ -2362,28 +2433,28 @@
       <c r="H86" s="2"/>
     </row>
     <row r="89" spans="1:8">
-      <c r="A89" s="22" t="s">
+      <c r="A89" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B89" s="22"/>
-      <c r="C89" s="22"/>
-      <c r="D89" s="22"/>
-      <c r="E89" s="22"/>
-      <c r="F89" s="22"/>
-      <c r="G89" s="22"/>
-      <c r="H89" s="22"/>
+      <c r="B89" s="15"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="15"/>
+      <c r="G89" s="15"/>
+      <c r="H89" s="15"/>
     </row>
     <row r="92" spans="1:8">
-      <c r="A92" s="15" t="s">
+      <c r="A92" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B92" s="16"/>
-      <c r="C92" s="16"/>
-      <c r="D92" s="16"/>
-      <c r="E92" s="16"/>
-      <c r="F92" s="16"/>
-      <c r="G92" s="16"/>
-      <c r="H92" s="16"/>
+      <c r="B92" s="17"/>
+      <c r="C92" s="17"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="17"/>
+      <c r="H92" s="17"/>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" s="7">
@@ -2444,16 +2515,16 @@
       <c r="H95" s="2"/>
     </row>
     <row r="97" spans="1:8">
-      <c r="A97" s="15" t="s">
+      <c r="A97" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B97" s="16"/>
-      <c r="C97" s="16"/>
-      <c r="D97" s="16"/>
-      <c r="E97" s="16"/>
-      <c r="F97" s="16"/>
-      <c r="G97" s="16"/>
-      <c r="H97" s="16"/>
+      <c r="B97" s="17"/>
+      <c r="C97" s="17"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="17"/>
+      <c r="F97" s="17"/>
+      <c r="G97" s="17"/>
+      <c r="H97" s="17"/>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" s="7">
@@ -2515,6 +2586,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A50:H50"/>
+    <mergeCell ref="A56:H56"/>
     <mergeCell ref="A89:H89"/>
     <mergeCell ref="A92:H92"/>
     <mergeCell ref="A97:H97"/>
@@ -2522,17 +2604,6 @@
     <mergeCell ref="A68:H68"/>
     <mergeCell ref="A74:H74"/>
     <mergeCell ref="A81:H81"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A50:H50"/>
-    <mergeCell ref="A56:H56"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A14:A19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2545,12 +2616,12 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="8" width="8.58203125" style="10"/>
+    <col min="1" max="8" width="8.625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2569,8 +2640,8 @@
       <c r="E1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>32</v>
+      <c r="F1" s="26" t="s">
+        <v>88</v>
       </c>
       <c r="G1" s="7">
         <v>80</v>
@@ -2656,8 +2727,8 @@
       <c r="E5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>46</v>
+      <c r="F5" s="26" t="s">
+        <v>89</v>
       </c>
       <c r="G5" s="7">
         <v>70</v>
@@ -2743,8 +2814,8 @@
       <c r="E9" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>50</v>
+      <c r="F9" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="G9" s="7">
         <v>30</v>
@@ -2830,8 +2901,8 @@
       <c r="E13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>56</v>
+      <c r="F13" s="26" t="s">
+        <v>91</v>
       </c>
       <c r="G13" s="7">
         <v>40</v>
@@ -2917,8 +2988,8 @@
       <c r="E17" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>57</v>
+      <c r="F17" s="26" t="s">
+        <v>92</v>
       </c>
       <c r="G17" s="7">
         <v>45</v>
@@ -3004,8 +3075,8 @@
       <c r="E21" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>58</v>
+      <c r="F21" s="26" t="s">
+        <v>93</v>
       </c>
       <c r="G21" s="7">
         <v>50</v>
@@ -3091,8 +3162,8 @@
       <c r="E25" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>72</v>
+      <c r="F25" s="26" t="s">
+        <v>94</v>
       </c>
       <c r="G25" s="7">
         <v>60</v>
@@ -3124,7 +3195,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:9" ht="34">
+    <row r="27" spans="1:9" ht="33">
       <c r="A27" s="4">
         <v>2</v>
       </c>
@@ -3196,8 +3267,8 @@
       <c r="E30" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="7" t="s">
-        <v>39</v>
+      <c r="F30" s="26" t="s">
+        <v>95</v>
       </c>
       <c r="G30" s="7">
         <v>70</v>
@@ -3296,13 +3367,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A38EC5C-4514-4B72-A7E2-347F92EED1EC}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="8" width="8.58203125" style="10"/>
+    <col min="1" max="5" width="8.625" style="10"/>
+    <col min="6" max="6" width="9" style="10"/>
+    <col min="7" max="8" width="8.625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3321,8 +3394,8 @@
       <c r="E1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>32</v>
+      <c r="F1" s="26" t="s">
+        <v>88</v>
       </c>
       <c r="G1" s="7">
         <v>80</v>
@@ -3408,8 +3481,8 @@
       <c r="E5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>46</v>
+      <c r="F5" s="26" t="s">
+        <v>89</v>
       </c>
       <c r="G5" s="7">
         <v>70</v>
@@ -3495,8 +3568,8 @@
       <c r="E9" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>50</v>
+      <c r="F9" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="G9" s="7">
         <v>30</v>
@@ -3582,8 +3655,8 @@
       <c r="E13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>56</v>
+      <c r="F13" s="26" t="s">
+        <v>91</v>
       </c>
       <c r="G13" s="7">
         <v>40</v>
@@ -3669,8 +3742,8 @@
       <c r="E17" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>57</v>
+      <c r="F17" s="26" t="s">
+        <v>92</v>
       </c>
       <c r="G17" s="7">
         <v>45</v>
@@ -3756,8 +3829,8 @@
       <c r="E21" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>58</v>
+      <c r="F21" s="26" t="s">
+        <v>93</v>
       </c>
       <c r="G21" s="7">
         <v>50</v>
@@ -3843,8 +3916,8 @@
       <c r="E25" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>72</v>
+      <c r="F25" s="26" t="s">
+        <v>94</v>
       </c>
       <c r="G25" s="7">
         <v>60</v>
@@ -3876,7 +3949,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:9" ht="34">
+    <row r="27" spans="1:9" ht="33">
       <c r="A27" s="4">
         <v>2</v>
       </c>
@@ -3948,8 +4021,8 @@
       <c r="E30" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="7" t="s">
-        <v>39</v>
+      <c r="F30" s="26" t="s">
+        <v>95</v>
       </c>
       <c r="G30" s="7">
         <v>70</v>
@@ -4039,28 +4112,28 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="7">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B35" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>46</v>
+        <v>96</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>97</v>
       </c>
       <c r="G35" s="7">
-        <v>70</v>
+        <v>4444</v>
       </c>
       <c r="H35" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I35">
         <v>9</v>
@@ -4068,21 +4141,20 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="4">
-        <v>400</v>
+        <v>4444</v>
       </c>
       <c r="B36" s="4">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C36" s="4">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D36" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E36" s="4">
         <v>2</v>
       </c>
-      <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
@@ -4102,25 +4174,23 @@
       <c r="E37" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="4">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="B38" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C38" s="4">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D38" s="4">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
@@ -4135,13 +4205,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A6246A-9F7B-4896-8792-1C606A73A571}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="8" width="8.58203125" style="10"/>
+    <col min="1" max="8" width="8.625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4152,16 +4222,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>77</v>
+      <c r="F1" s="26" t="s">
+        <v>104</v>
       </c>
       <c r="G1" s="7">
         <v>120</v>
@@ -4194,11 +4264,11 @@
       <c r="B3" s="2">
         <v>0.5</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>81</v>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -4213,16 +4283,16 @@
         <v>0</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>80</v>
+      <c r="F4" s="26" t="s">
+        <v>105</v>
       </c>
       <c r="G4" s="7">
         <v>150</v>
@@ -4255,11 +4325,11 @@
       <c r="B6" s="2">
         <v>0.5</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>81</v>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>

</xml_diff>